<commit_message>
Finished the dynamic row drill
</commit_message>
<xml_diff>
--- a/DynamicTotalRow.xlsx
+++ b/DynamicTotalRow.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{B55FA4AD-2961-4C14-B55E-345C4EEA53E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC72346B-9F75-47F4-8495-05A52947B43B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
+    <sheet name="Alt2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_c" localSheetId="1">'Alt2'!$G$4</definedName>
     <definedName name="_c">Report!$G$2</definedName>
     <definedName name="HD_Date">_xlfn.LET(_xlpm.dt, TODAY(),      _xlpm.y,  YEAR(_xlpm.dt),      _xlpm.m,  MONTH(_xlpm.dt),      _xlpm.d,  DAY(_xlpm.dt),      TEXT(DATE(_xlpm.y,_xlpm.m,_xlpm.d),"dd-mmm-yyyy")     )</definedName>
   </definedNames>
@@ -31,6 +33,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -60,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="20">
   <si>
     <t>Value</t>
   </si>
@@ -108,6 +112,18 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=vmSkRbS3fTA</t>
+  </si>
+  <si>
+    <t>Total Row:</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>SUM</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -306,7 +322,7 @@
     <cellStyle name="Title" xfId="1" builtinId="15" hidden="1"/>
     <cellStyle name="Total" xfId="6" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="23">
     <dxf>
       <fill>
         <patternFill>
@@ -329,6 +345,32 @@
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -565,27 +607,27 @@
   </dxfs>
   <tableStyles count="2" defaultTableStyle="Biegert Table Standard" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Biegert Standard Pivot Table" table="0" count="12" xr9:uid="{94886349-6B4A-4300-89B0-9F83C8B5183A}">
-      <tableStyleElement type="wholeTable" dxfId="20"/>
-      <tableStyleElement type="headerRow" dxfId="19"/>
-      <tableStyleElement type="totalRow" dxfId="18"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="17"/>
-      <tableStyleElement type="firstHeaderCell" dxfId="16"/>
-      <tableStyleElement type="firstSubtotalColumn" dxfId="15"/>
-      <tableStyleElement type="firstSubtotalRow" dxfId="14"/>
-      <tableStyleElement type="secondSubtotalRow" dxfId="13"/>
-      <tableStyleElement type="firstRowSubheading" dxfId="12"/>
-      <tableStyleElement type="secondRowSubheading" dxfId="11"/>
-      <tableStyleElement type="pageFieldLabels" dxfId="10"/>
-      <tableStyleElement type="pageFieldValues" dxfId="9"/>
+      <tableStyleElement type="wholeTable" dxfId="22"/>
+      <tableStyleElement type="headerRow" dxfId="21"/>
+      <tableStyleElement type="totalRow" dxfId="20"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="19"/>
+      <tableStyleElement type="firstHeaderCell" dxfId="18"/>
+      <tableStyleElement type="firstSubtotalColumn" dxfId="17"/>
+      <tableStyleElement type="firstSubtotalRow" dxfId="16"/>
+      <tableStyleElement type="secondSubtotalRow" dxfId="15"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="14"/>
+      <tableStyleElement type="secondRowSubheading" dxfId="13"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="12"/>
+      <tableStyleElement type="pageFieldValues" dxfId="11"/>
     </tableStyle>
     <tableStyle name="Biegert Table Standard" pivot="0" count="7" xr9:uid="{95B43237-2845-4068-A415-A5A3E7804959}">
-      <tableStyleElement type="wholeTable" dxfId="8"/>
-      <tableStyleElement type="headerRow" dxfId="7"/>
-      <tableStyleElement type="totalRow" dxfId="6"/>
-      <tableStyleElement type="firstColumn" dxfId="5"/>
-      <tableStyleElement type="lastColumn" dxfId="4"/>
-      <tableStyleElement type="firstRowStripe" dxfId="3"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="2"/>
+      <tableStyleElement type="wholeTable" dxfId="10"/>
+      <tableStyleElement type="headerRow" dxfId="9"/>
+      <tableStyleElement type="totalRow" dxfId="8"/>
+      <tableStyleElement type="firstColumn" dxfId="7"/>
+      <tableStyleElement type="lastColumn" dxfId="6"/>
+      <tableStyleElement type="firstRowStripe" dxfId="5"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="4"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -608,14 +650,103 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>403860</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Speech Bubble: Oval 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28F5631C-C420-2FAD-D46B-0BD6D360535A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8488680" y="701040"/>
+          <a:ext cx="1455420" cy="1074420"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeEllipseCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -164288"/>
+            <a:gd name="adj2" fmla="val -85635"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200"/>
+            <a:t>Must contain</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200" baseline="0"/>
+            <a:t> a space for no function</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" kern="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8AE4C564-EC9B-400B-B900-DAD794C67EDE}" name="Data" displayName="Data" ref="A1:D14" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8AE4C564-EC9B-400B-B900-DAD794C67EDE}" name="Data" displayName="Data" ref="A1:D14" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A1:D14" xr:uid="{8AE4C564-EC9B-400B-B900-DAD794C67EDE}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{B696CCE1-59F9-4EF9-B93B-CAF341686250}" name="Item"/>
     <tableColumn id="2" xr3:uid="{D1D6F669-C2E5-4AB3-9658-F68AF9147F4A}" name="Units"/>
     <tableColumn id="3" xr3:uid="{D43E33A2-892A-47B4-B7A3-51B21BA5B3D7}" name="Region"/>
     <tableColumn id="4" xr3:uid="{D8FF9AA5-E20D-4541-9564-5B65502A3873}" name="Value"/>
+  </tableColumns>
+  <tableStyleInfo name="Biegert Table Standard" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7F342EE3-AA99-4E07-8717-5FF1DC77B551}" name="Data2" displayName="Data2" ref="A1:D14" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:D14" xr:uid="{8AE4C564-EC9B-400B-B900-DAD794C67EDE}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{F23F9FFC-07D2-402C-B493-14B6002C6E90}" name="Item"/>
+    <tableColumn id="2" xr3:uid="{825BCFCA-0F89-46CA-9780-ED3537756438}" name="Units"/>
+    <tableColumn id="3" xr3:uid="{D8F65625-C098-4377-92B6-55721F126100}" name="Region"/>
+    <tableColumn id="4" xr3:uid="{CF8DA6F7-E642-4FB9-ADAD-8D4306582BE5}" name="Value"/>
   </tableColumns>
   <tableStyleInfo name="Biegert Table Standard" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -813,8 +944,8 @@
   </sheetPr>
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1115,7 +1246,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F5:I26">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>$F5="Total"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1125,4 +1256,341 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CD51DDA-0330-4C51-9EFC-E0532B4E4014}">
+  <sheetPr>
+    <tabColor rgb="FFCCFFCC"/>
+  </sheetPr>
+  <dimension ref="A1:L14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="7.88671875" customWidth="1"/>
+    <col min="5" max="5" width="9" customWidth="1"/>
+    <col min="6" max="9" width="14.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>71</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2">
+        <v>174.66</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>37</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>91.02</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>54</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <v>132.84</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>58</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>142.68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>63</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <v>154.97999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>44</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <v>108.24</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>76</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8">
+        <v>186.96</v>
+      </c>
+      <c r="F8" t="str" cm="1">
+        <f t="array" ref="F8:I12">_xlfn.LET(
+_xlpm.Array,_xlfn._xlws.FILTER(Data2[],Data2[Item]=_c,{"","","",""}),
+_xlpm.CalcType, _xlfn.SWITCH(G2:J2,"SUM",_xleta.SUM,"COUNTA",_xleta.COUNTA,"AVERAGE",_xleta.AVERAGE,G2:J2),
+_xlpm.ColIndex, _xlfn.SEQUENCE(1,COLUMNS(_xlpm.CalcType)),
+_xlpm.TotalCalc, _xlfn.MAP(_xlpm.ColIndex,_xlfn.LAMBDA(_xlpm.v,_xlfn.BYCOL(_xlfn.CHOOSECOLS(_xlpm.Array,_xlpm.v),_xlfn.CHOOSECOLS(_xlpm.CalcType,_xlpm.v)))),
+_xlpm.TotalRow,IF(ISTEXT(_xlpm.CalcType),_xlpm.CalcType,_xlpm.TotalCalc),
+_xlpm.Result,_xlfn.VSTACK(_xlpm.Array,_xlpm.TotalRow),
+_xlpm.Result
+)</f>
+        <v>Alpha</v>
+      </c>
+      <c r="G8">
+        <v>71</v>
+      </c>
+      <c r="H8" t="str">
+        <v>North</v>
+      </c>
+      <c r="I8">
+        <v>174.66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9">
+        <v>68.88</v>
+      </c>
+      <c r="F9" t="str">
+        <v>Alpha</v>
+      </c>
+      <c r="G9">
+        <v>58</v>
+      </c>
+      <c r="H9" t="str">
+        <v>South</v>
+      </c>
+      <c r="I9">
+        <v>142.68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>67</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10">
+        <v>164.82</v>
+      </c>
+      <c r="F10" t="str">
+        <v>Alpha</v>
+      </c>
+      <c r="G10">
+        <v>76</v>
+      </c>
+      <c r="H10" t="str">
+        <v>East</v>
+      </c>
+      <c r="I10">
+        <v>186.96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11">
+        <v>43</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11">
+        <v>105.78</v>
+      </c>
+      <c r="F11" t="str">
+        <v>Alpha</v>
+      </c>
+      <c r="G11">
+        <v>43</v>
+      </c>
+      <c r="H11" t="str">
+        <v>West</v>
+      </c>
+      <c r="I11">
+        <v>105.78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>57</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12">
+        <v>140.22</v>
+      </c>
+      <c r="F12" t="str">
+        <v>Total</v>
+      </c>
+      <c r="G12">
+        <v>248</v>
+      </c>
+      <c r="H12" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="I12">
+        <v>610.08000000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>68</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13">
+        <v>167.28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>49</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14">
+        <v>120.54</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="F8:I26">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$F8="Total"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>